<commit_message>
Sommaire et plan bien avancé
</commit_message>
<xml_diff>
--- a/REAC_Comp.xlsx
+++ b/REAC_Comp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AY024303\Cyril\Doc perso\Diplome I5\Dossier-proj\Info dossier pro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril\DossierPerso\Document Important\école sup\Dossier_prof\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93B8AC-3D0E-4A6F-B3C5-9D34E2085A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8B022D-E19D-446E-A88F-741E4A4BFF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{B7C02CEF-25C9-4280-8BD4-DADB43DFD29C}"/>
+    <workbookView xWindow="28680" yWindow="-4680" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B7C02CEF-25C9-4280-8BD4-DADB43DFD29C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="245">
   <si>
     <t>A2T2S3 – Management des processus S.I.</t>
   </si>
@@ -456,9 +456,6 @@
   </si>
   <si>
     <t>Conduire le changement auprès des métiers lors du déploiement d’une solution applicative ou intégrée en mettant en place une démarche de participation, de communication et de formation pour accompagner les utilisateurs à l’intégration du nouvel outil dans leurs habitudes de travail</t>
-  </si>
-  <si>
-    <t>BC01 – Analyser et définir la stratégie d’un système d’information</t>
   </si>
   <si>
     <t>PSSI de Ausy : comment il gère les accès de droit
@@ -481,24 +478,11 @@
 demander au chef de projet les KPA</t>
   </si>
   <si>
-    <t>Outil managérial 
-voir les critères de choix qui plait à Domus et pourquoi tel personne est bien pour cette mission (en  se plaçant d'Ausy)
-pas obliger de répondre</t>
-  </si>
-  <si>
     <t>Demander à mon entreprise :
 Savoir s'ils ont un projet
 passer de server à cloud =&gt; RSE</t>
   </si>
   <si>
-    <t>Demande à Ausy
-Permet de faire le liena vec Domsuvi
-parler du lien avec eux</t>
-  </si>
-  <si>
-    <t>BC02 – Manager un projet informatique avec agilité en collaboration avec les parties prenantes</t>
-  </si>
-  <si>
     <t>Identifier l’ensemble des étapes de réalisation du système d’information pour organiser le projet en tâches et livrables en répartissant les activités en fonction des ressources humaines, techniques et financières à mobiliser</t>
   </si>
   <si>
@@ -532,23 +516,313 @@
     <t>explication de comment je ressens le teletravail</t>
   </si>
   <si>
-    <t>BC03 – Piloter l’informatique décisionnelle d’un S.I. (big data &amp; business intelligence)</t>
-  </si>
-  <si>
     <t>Définir les données de référence de l’entreprise à partir des données utilisées pour créer un référentiel de données afin d’assurer la mise à disposition de données cohérentes aux directions métiers</t>
   </si>
   <si>
-    <t>BC04 – Concevoir et développer des solutions applicatives métier et spécifiques (mobiles, embarquées et ERP)</t>
-  </si>
-  <si>
     <t>Collecter les besoins métiers des utilisateurs en menant des interviews auprès d’eux pour comprendre leurs activités et leurs contraintes métier afin d’étudier les opportunités et la faisabilité technologique d’une solution applicative spécifique ou métier.</t>
+  </si>
+  <si>
+    <t>Projet MSAL : Demande Anis
+Etudes Technique ?</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>= &gt;</t>
+  </si>
+  <si>
+    <t>Besoin de la PSSI : avec info sur l'accès aux données (droits), l'intégrité (save, repair), disponibilité (SLA), gestion risques</t>
+  </si>
+  <si>
+    <t>l’environnement économique , l’activité métier de l’entreprise, les parties prenantes
+-la gestion stratégie, opérationnelle et techno du S.I., le SI et les acteurs
+analyse et synthétise par écrit son diagnostic. présente ses préconisations</t>
+  </si>
+  <si>
+    <t>Projet CRM 3.0 (new graphisme) nouvelle pagination, nouvelle fonctionnalité
+Projet CRM 4.0/ICD ?
+Projet TMA ?</t>
+  </si>
+  <si>
+    <t>SWOT sur AUSY (voire Domusvi si motivé)</t>
+  </si>
+  <si>
+    <t>Moi solo +
+Info à voir avec Amine</t>
+  </si>
+  <si>
+    <t>PTDR : NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outil managérial 
+voir les critères de choix qui plait à Domus et pourquoi tel personne est bien pour cette mission (en  se plaçant d'Ausy)
+</t>
+  </si>
+  <si>
+    <t>Demande à Ausy
+Permet de faire le lien avec Domsuvi
+parler du lien avec eux</t>
+  </si>
+  <si>
+    <t>Info à voir avec Amine</t>
+  </si>
+  <si>
+    <t>SLA en général demadner SLA Ausy-Domusvi
+Norme au Sein du SI (ISO, ITIL, GREEN, …)</t>
+  </si>
+  <si>
+    <t>Info à voir avec Amine/Olivier/Damien
+Demadner à Laurent/Aurélien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info sur les personnes qu'a proposer Ausy
+Critère : Com ? Riqueur ? (Ali qui est de Lille)
+Parler de ce qu'il leur plaît chez moi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projet Green, RSE ? Sinon à qui demander </t>
+  </si>
+  <si>
+    <t>Info à voir avec Amine/Landry</t>
+  </si>
+  <si>
+    <t>logiciel BPM : entités externes, processus, données et flux</t>
+  </si>
+  <si>
+    <t>Info à voir avec Amine/Landry ?</t>
+  </si>
+  <si>
+    <t>Projet ICD ? Info avec les Diag, test fonc …
+!! On est en API mnt (pas FTP), parler de pk on a changé</t>
+  </si>
+  <si>
+    <t>En agile CDC = Backlog + projet ICD</t>
+  </si>
+  <si>
+    <t>Agile</t>
+  </si>
+  <si>
+    <t>Agile + Info sur les indicateurs (vélocité, nb bug, …)</t>
+  </si>
+  <si>
+    <t>Info Hana/Laurent</t>
+  </si>
+  <si>
+    <t>MSPR ??</t>
+  </si>
+  <si>
+    <t>Discussion ouverte après DSM, visite Paris-Lyon</t>
+  </si>
+  <si>
+    <t>NA : Juste bon sens</t>
+  </si>
+  <si>
+    <t>Liste des logiciels d'échanges : discord, Teams, Azure, réunion (Start Week, Démo, Pres projet...)
+Avec la liste des moyens de communications, reste en contact</t>
+  </si>
+  <si>
+    <t>Parler des dérogation de Télétravail, de gain de productiivité vue (temps com ++, fréquence de com --, moins solicité en télétravail)</t>
+  </si>
+  <si>
+    <t>Projet ICD
+Projet CRM3.0 (4.0 aussi ?)</t>
+  </si>
+  <si>
+    <t>une démonstration technique de son application (interprétation de certaines lignes de codes)</t>
+  </si>
+  <si>
+    <t>Projet CRM …
+Projet CAC (gestion des chevauchement RDV)</t>
+  </si>
+  <si>
+    <t>Projet ICD/CAC
+Mission Portal en géné (micro appli)</t>
+  </si>
+  <si>
+    <t>Projet MSAL : plan de test</t>
+  </si>
+  <si>
+    <t>Azure DevOps</t>
+  </si>
+  <si>
+    <t>Question pour Laurent</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NA on fait pas de Doc ...</t>
+  </si>
+  <si>
+    <t>Comment les métier vivent les chgts et ajout de fonctionnalités ? Question Laurent</t>
+  </si>
+  <si>
+    <t>NA : Les métiers demandent les chgt</t>
+  </si>
+  <si>
+    <t>MSPR BIG DATA : Gestion des données
+Schéma flux (BPM ?)</t>
+  </si>
+  <si>
+    <t>MSPR BIG DATA : Techno et outils</t>
+  </si>
+  <si>
+    <t>MSPR Big Data : remplissage DT (+ieurs sources, +ieurs BDD prod)</t>
+  </si>
+  <si>
+    <t>NA : Inventer prédiction, prévisions ?</t>
+  </si>
+  <si>
+    <t>PowerBI : avec Dahsboard Mensuel</t>
+  </si>
+  <si>
+    <t>Analyse  de l'entreprise et de leurs besoins en terme de donées, validation données</t>
+  </si>
+  <si>
+    <t>NA : PTTDR c'est quoi</t>
+  </si>
+  <si>
+    <t>Outil de nettoyage de données (Power BI)</t>
+  </si>
+  <si>
+    <t>RSSI et RDPG</t>
+  </si>
+  <si>
+    <t>A3C2</t>
+  </si>
+  <si>
+    <t>A3C1</t>
+  </si>
+  <si>
+    <t>A3C3</t>
+  </si>
+  <si>
+    <t>A3C4</t>
+  </si>
+  <si>
+    <t>A3C5</t>
+  </si>
+  <si>
+    <t>A3C6</t>
+  </si>
+  <si>
+    <t>A3C7</t>
+  </si>
+  <si>
+    <t>A3C8</t>
+  </si>
+  <si>
+    <t>A2C1</t>
+  </si>
+  <si>
+    <t>A2C2</t>
+  </si>
+  <si>
+    <t>A2C3</t>
+  </si>
+  <si>
+    <t>A2C4</t>
+  </si>
+  <si>
+    <t>A2C5</t>
+  </si>
+  <si>
+    <t>A2C6</t>
+  </si>
+  <si>
+    <t>A2C7</t>
+  </si>
+  <si>
+    <t>A2C8</t>
+  </si>
+  <si>
+    <t>A1 – Analyse et définition de la stratégie des systèmes d’information</t>
+  </si>
+  <si>
+    <t>A1C1</t>
+  </si>
+  <si>
+    <t>A1C2</t>
+  </si>
+  <si>
+    <t>A1C4</t>
+  </si>
+  <si>
+    <t>A1C3</t>
+  </si>
+  <si>
+    <t>A1C5</t>
+  </si>
+  <si>
+    <t>A1C6</t>
+  </si>
+  <si>
+    <t>A1C7</t>
+  </si>
+  <si>
+    <t>A4C1</t>
+  </si>
+  <si>
+    <t>A4C2</t>
+  </si>
+  <si>
+    <t>A4C3</t>
+  </si>
+  <si>
+    <t>A4C5</t>
+  </si>
+  <si>
+    <t>A4C4</t>
+  </si>
+  <si>
+    <t>A4C6</t>
+  </si>
+  <si>
+    <t>A4C7</t>
+  </si>
+  <si>
+    <t>A4C8</t>
+  </si>
+  <si>
+    <t>A4C9</t>
+  </si>
+  <si>
+    <t>A4 – Pilotage de l’informatique décisionnelle d’un système d’information (business intelligence &amp; big data)</t>
+  </si>
+  <si>
+    <t>A5C1</t>
+  </si>
+  <si>
+    <t>A5C2</t>
+  </si>
+  <si>
+    <t>A5C3</t>
+  </si>
+  <si>
+    <t>A5C4</t>
+  </si>
+  <si>
+    <t>A5C5</t>
+  </si>
+  <si>
+    <t>A5C6</t>
+  </si>
+  <si>
+    <t>A5C8</t>
+  </si>
+  <si>
+    <t>A5C7</t>
+  </si>
+  <si>
+    <t>Contexte de la mission/ Analyse du context</t>
+  </si>
+  <si>
+    <t>MAIS en vrai parler des choses à améliorer dans l'équipes ? (rédaction US, TMA, …)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,6 +858,79 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -599,7 +946,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -1208,21 +1555,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -1232,12 +1564,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1250,9 +1621,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1262,18 +1631,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="double">
@@ -1286,7 +1644,18 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="double">
@@ -1296,11 +1665,37 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1309,7 +1704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1371,6 +1766,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1404,176 +1832,257 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1590,6 +2099,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2783540</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>587828</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>18680</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>475192</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE2E8654-5B53-2508-7EF1-85A3A73B1F6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11415911" y="587828"/>
+          <a:ext cx="7829390" cy="3988013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1891,22 +2455,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64E06A1-5828-401C-8B0D-EF32609AE8B1}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="B30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:C25"/>
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="23.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="40.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="48.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40.5546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="45" style="20" customWidth="1"/>
-    <col min="4" max="4" width="76.54296875" style="32" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="39.1796875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.54296875" style="1"/>
+    <col min="4" max="4" width="76.5546875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="39.21875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>64</v>
       </c>
@@ -1916,7 +2480,7 @@
       <c r="C1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="32" t="s">
         <v>67</v>
       </c>
       <c r="E1" s="11" t="s">
@@ -1926,8 +2490,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="59" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="60" t="s">
+    <row r="2" spans="1:6" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="69" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1936,7 +2500,7 @@
       <c r="C2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="33" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -1946,15 +2510,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="98.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="60"/>
-      <c r="B3" s="62" t="s">
+    <row r="3" spans="1:6" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="69"/>
+      <c r="B3" s="71" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="34" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="12" t="s">
@@ -1964,13 +2528,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="60"/>
-      <c r="B4" s="63"/>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="69"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="35" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="12" t="s">
@@ -1978,13 +2542,13 @@
       </c>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="60"/>
-      <c r="B5" s="63"/>
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="69"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="35" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -1992,13 +2556,13 @@
       </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="60"/>
-      <c r="B6" s="64"/>
+    <row r="6" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="69"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="36" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="12" t="s">
@@ -2006,15 +2570,15 @@
       </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="60"/>
-      <c r="B7" s="62" t="s">
+    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="69"/>
+      <c r="B7" s="71" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="37" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="12" t="s">
@@ -2022,39 +2586,39 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="43.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="60"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="74" t="s">
+    <row r="8" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="69"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="78"/>
-    </row>
-    <row r="9" spans="1:6" ht="21.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="61"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="78"/>
-    </row>
-    <row r="10" spans="1:6" ht="44" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="70" t="s">
+      <c r="F8" s="87"/>
+    </row>
+    <row r="9" spans="1:6" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="70"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="87"/>
+    </row>
+    <row r="10" spans="1:6" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="39" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="12" t="s">
@@ -2064,11 +2628,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="60"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="24" t="s">
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="69"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="35" t="s">
         <v>50</v>
       </c>
       <c r="E11" s="12" t="s">
@@ -2078,13 +2642,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="60"/>
-      <c r="B12" s="67"/>
+    <row r="12" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="69"/>
+      <c r="B12" s="76"/>
       <c r="C12" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="36" t="s">
         <v>52</v>
       </c>
       <c r="E12" s="12" t="s">
@@ -2094,15 +2658,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A13" s="60"/>
-      <c r="B13" s="71" t="s">
+    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="69"/>
+      <c r="B13" s="80" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="34" t="s">
         <v>55</v>
       </c>
       <c r="E13" s="12" t="s">
@@ -2112,13 +2676,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="60"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="69" t="s">
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="69"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="35" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="12" t="s">
@@ -2128,11 +2692,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="60"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="24" t="s">
+    <row r="15" spans="1:6" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="69"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="35" t="s">
         <v>58</v>
       </c>
       <c r="E15" s="12" t="s">
@@ -2142,11 +2706,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="60"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="24" t="s">
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="69"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="35" t="s">
         <v>59</v>
       </c>
       <c r="E16" s="12" t="s">
@@ -2156,13 +2720,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="61"/>
-      <c r="B17" s="66"/>
+    <row r="17" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="70"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="12" t="s">
@@ -2172,15 +2736,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="57.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="37" t="s">
+    <row r="18" spans="1:6" ht="57.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="23" t="s">
+      <c r="C18" s="62"/>
+      <c r="D18" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="12" t="s">
@@ -2190,11 +2754,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="38"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="27" t="s">
+    <row r="19" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="47"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="12" t="s">
@@ -2204,13 +2768,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="86.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="38"/>
-      <c r="B20" s="58" t="s">
+    <row r="20" spans="1:6" ht="86.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="47"/>
+      <c r="B20" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="29" t="s">
+      <c r="C20" s="68"/>
+      <c r="D20" s="40" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="12" t="s">
@@ -2220,23 +2784,23 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="101.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="38"/>
-      <c r="B21" s="40" t="s">
+    <row r="21" spans="1:6" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="47"/>
+      <c r="B21" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="23" t="s">
+      <c r="C21" s="50"/>
+      <c r="D21" s="34" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="38"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="24" t="s">
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="47"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="35" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="12" t="s">
@@ -2246,11 +2810,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="38"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="24" t="s">
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="47"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="35" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="12" t="s">
@@ -2260,11 +2824,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="38"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="24" t="s">
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="47"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="35" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="12" t="s">
@@ -2274,11 +2838,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="39"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="30" t="s">
+    <row r="25" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="48"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="41" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="12" t="s">
@@ -2288,15 +2852,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="36" t="s">
+    <row r="26" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="28" t="s">
+      <c r="C26" s="56"/>
+      <c r="D26" s="39" t="s">
         <v>89</v>
       </c>
       <c r="E26" s="12" t="s">
@@ -2306,11 +2870,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="34"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="24" t="s">
+    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="43"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="35" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="12" t="s">
@@ -2320,11 +2884,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="34"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="25" t="s">
+    <row r="28" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="43"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="36" t="s">
         <v>17</v>
       </c>
       <c r="E28" s="12" t="s">
@@ -2334,13 +2898,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="34"/>
-      <c r="B29" s="52" t="s">
+    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="43"/>
+      <c r="B29" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="53"/>
-      <c r="D29" s="23" t="s">
+      <c r="C29" s="62"/>
+      <c r="D29" s="34" t="s">
         <v>19</v>
       </c>
       <c r="E29" s="12" t="s">
@@ -2348,11 +2912,11 @@
       </c>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="34"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="25" t="s">
+    <row r="30" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="43"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="36" t="s">
         <v>20</v>
       </c>
       <c r="E30" s="12" t="s">
@@ -2362,13 +2926,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="34"/>
-      <c r="B31" s="52" t="s">
+    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="43"/>
+      <c r="B31" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="53"/>
-      <c r="D31" s="23" t="s">
+      <c r="C31" s="62"/>
+      <c r="D31" s="34" t="s">
         <v>22</v>
       </c>
       <c r="E31" s="12" t="s">
@@ -2378,11 +2942,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="34"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="25" t="s">
+    <row r="32" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="43"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="36" t="s">
         <v>23</v>
       </c>
       <c r="E32" s="12" t="s">
@@ -2392,13 +2956,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="34"/>
-      <c r="B33" s="52" t="s">
+    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="43"/>
+      <c r="B33" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="23" t="s">
+      <c r="C33" s="62"/>
+      <c r="D33" s="34" t="s">
         <v>25</v>
       </c>
       <c r="E33" s="12" t="s">
@@ -2406,11 +2970,11 @@
       </c>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="35"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="30" t="s">
+    <row r="34" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="44"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="41" t="s">
         <v>26</v>
       </c>
       <c r="E34" s="12" t="s">
@@ -2420,15 +2984,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="34" t="s">
+    <row r="35" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="31" t="s">
+      <c r="C35" s="52"/>
+      <c r="D35" s="42" t="s">
         <v>29</v>
       </c>
       <c r="E35" s="12" t="s">
@@ -2438,11 +3002,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="34"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="24" t="s">
+    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="43"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="35" t="s">
         <v>30</v>
       </c>
       <c r="E36" s="12" t="s">
@@ -2452,11 +3016,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="34"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="24" t="s">
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="43"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="35" t="s">
         <v>31</v>
       </c>
       <c r="E37" s="12" t="s">
@@ -2466,21 +3030,21 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="35"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="30" t="s">
+    <row r="38" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="44"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="33" t="s">
+      <c r="E38" s="22" t="s">
         <v>72</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="24" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:6" ht="24" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
     <mergeCell ref="D8:D9"/>
@@ -2514,329 +3078,736 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D8D677-BCDB-47D5-ABA2-09C3D35E14AC}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="75.08984375" style="32" customWidth="1"/>
-    <col min="2" max="2" width="50.7265625" style="32" customWidth="1"/>
-    <col min="3" max="16384" width="10.90625" style="32"/>
+    <col min="1" max="1" width="92.77734375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="96" customWidth="1"/>
+    <col min="3" max="3" width="61.44140625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="40.5546875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="47.88671875" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="10.88671875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="93.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:13" ht="93.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="101" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="103"/>
+    </row>
+    <row r="2" spans="1:13" ht="59.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="122" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="122" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="122" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="84"/>
-    </row>
-    <row r="2" spans="1:2" ht="59.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="81" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="79"/>
-    </row>
-    <row r="3" spans="1:2" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="81" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="79"/>
-    </row>
-    <row r="4" spans="1:2" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="81" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="79"/>
-    </row>
-    <row r="5" spans="1:2" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="81" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="79" t="s">
+      <c r="E6" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="81.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="122" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" s="90" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="74" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="81" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="79" t="s">
+      <c r="E7" s="90" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="88.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="99" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="123" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="120" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="121" t="s">
+        <v>244</v>
+      </c>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+    </row>
+    <row r="9" spans="1:13" ht="60.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+    </row>
+    <row r="10" spans="1:13" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="109" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="106"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
+    </row>
+    <row r="11" spans="1:13" ht="83.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="93" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="90"/>
+    </row>
+    <row r="12" spans="1:13" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="93" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
+    </row>
+    <row r="13" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="93" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="105"/>
+    </row>
+    <row r="14" spans="1:13" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="93" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="90"/>
+    </row>
+    <row r="15" spans="1:13" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="93" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="81" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="79"/>
-    </row>
-    <row r="8" spans="1:2" ht="88" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="81" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="79" t="s">
+      <c r="D15" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="90"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="90"/>
+    </row>
+    <row r="16" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="93" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="90"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="90"/>
+    </row>
+    <row r="17" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="93" t="s">
+        <v>215</v>
+      </c>
+      <c r="C17" s="119" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="81" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="79" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="81" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="79" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="79" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="50.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="82" t="s">
+      <c r="D17" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="90"/>
+    </row>
+    <row r="18" spans="1:13" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="80"/>
-    </row>
-    <row r="13" spans="1:2" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="86"/>
-      <c r="B13" s="86"/>
-    </row>
-    <row r="14" spans="1:2" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="87" t="s">
+      <c r="B18" s="107" t="s">
+        <v>216</v>
+      </c>
+      <c r="C18" s="108" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="90"/>
+    </row>
+    <row r="19" spans="1:13" ht="72.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="90"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="90"/>
+      <c r="L19" s="94"/>
+      <c r="M19" s="90"/>
+    </row>
+    <row r="20" spans="1:13" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="110" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="111"/>
+      <c r="C20" s="112"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="90"/>
+      <c r="L20" s="94"/>
+      <c r="M20" s="90"/>
+    </row>
+    <row r="21" spans="1:13" ht="66.599999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="93" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="B14" s="85"/>
-    </row>
-    <row r="15" spans="1:2" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="81" t="s">
+      <c r="D21" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="90"/>
+      <c r="K21" s="90"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="90"/>
+    </row>
+    <row r="22" spans="1:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="B15" s="79" t="s">
+      <c r="D22" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="90"/>
+      <c r="K22" s="90"/>
+      <c r="L22" s="90"/>
+      <c r="M22" s="90"/>
+    </row>
+    <row r="23" spans="1:13" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="125" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="90"/>
+    </row>
+    <row r="24" spans="1:13" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="93" t="s">
+        <v>204</v>
+      </c>
+      <c r="C24" s="24" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="81" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="79" t="s">
+      <c r="D24" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="90"/>
+      <c r="L24" s="90"/>
+      <c r="M24" s="90"/>
+    </row>
+    <row r="25" spans="1:13" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="93" t="s">
+        <v>205</v>
+      </c>
+      <c r="C25" s="24" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="81" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" s="79"/>
-    </row>
-    <row r="18" spans="1:2" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="81" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18" s="79" t="s">
+      <c r="D25" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="90"/>
+    </row>
+    <row r="26" spans="1:13" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="93" t="s">
+        <v>206</v>
+      </c>
+      <c r="C26" s="24" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="81" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" s="79" t="s">
+      <c r="D26" s="94"/>
+    </row>
+    <row r="27" spans="1:13" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="93" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="24" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="81" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="79"/>
-    </row>
-    <row r="21" spans="1:2" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="81" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" s="79" t="s">
+      <c r="D27" s="94"/>
+      <c r="E27" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="99" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="107" t="s">
+        <v>208</v>
+      </c>
+      <c r="C28" s="108" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="81" t="s">
-        <v>117</v>
-      </c>
-      <c r="B22" s="79" t="s">
+      <c r="D28" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="91"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="28"/>
+    </row>
+    <row r="30" spans="1:13" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="88" t="s">
+        <v>234</v>
+      </c>
+      <c r="B30" s="92"/>
+      <c r="C30" s="89"/>
+      <c r="E30" s="28"/>
+    </row>
+    <row r="31" spans="1:13" ht="61.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="93" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="93" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="125" t="s">
+        <v>229</v>
+      </c>
+      <c r="C34" s="113" t="s">
+        <v>195</v>
+      </c>
+      <c r="D34" s="31"/>
+    </row>
+    <row r="35" spans="1:4" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="93" t="s">
+        <v>228</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="24" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" s="79" t="s">
+      <c r="B36" s="93" t="s">
+        <v>230</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" s="125" t="s">
+        <v>231</v>
+      </c>
+      <c r="C37" s="114" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" s="30"/>
+    </row>
+    <row r="38" spans="1:4" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="93" t="s">
+        <v>232</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="99" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="100" t="s">
+        <v>233</v>
+      </c>
+      <c r="C39" s="115" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="69" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="91"/>
+      <c r="B40" s="95"/>
+      <c r="C40" s="90"/>
+      <c r="D40" s="90"/>
+    </row>
+    <row r="41" spans="1:4" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="92"/>
+      <c r="C41" s="97"/>
+    </row>
+    <row r="42" spans="1:4" ht="66.599999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="24" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="81" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="79" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="81" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" s="79" t="s">
+      <c r="B42" s="93" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="98" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="93" t="s">
+        <v>236</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="93" t="s">
+        <v>237</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B45" s="125" t="s">
+        <v>238</v>
+      </c>
+      <c r="C45" s="116" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="82" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" s="80"/>
-    </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="28" spans="1:2" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="83" t="s">
-        <v>155</v>
-      </c>
-      <c r="B28" s="84"/>
-    </row>
-    <row r="29" spans="1:2" ht="44" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="81" t="s">
-        <v>122</v>
-      </c>
-      <c r="B29" s="79"/>
-    </row>
-    <row r="30" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="81" t="s">
-        <v>123</v>
-      </c>
-      <c r="B30" s="79"/>
-    </row>
-    <row r="31" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="81" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" s="79"/>
-    </row>
-    <row r="32" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="81" t="s">
-        <v>125</v>
-      </c>
-      <c r="B32" s="79"/>
-    </row>
-    <row r="33" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="81" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" s="79"/>
-    </row>
-    <row r="34" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="81" t="s">
-        <v>156</v>
-      </c>
-      <c r="B34" s="79"/>
-    </row>
-    <row r="35" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="81" t="s">
-        <v>127</v>
-      </c>
-      <c r="B35" s="79"/>
-    </row>
-    <row r="36" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="81" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="79"/>
-    </row>
-    <row r="37" spans="1:2" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="82" t="s">
-        <v>129</v>
-      </c>
-      <c r="B37" s="80"/>
-    </row>
-    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="86"/>
-      <c r="B38" s="88"/>
-    </row>
-    <row r="39" spans="1:2" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="83" t="s">
-        <v>157</v>
-      </c>
-      <c r="B39" s="84"/>
-    </row>
-    <row r="40" spans="1:2" ht="46.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="81" t="s">
-        <v>158</v>
-      </c>
-      <c r="B40" s="79"/>
-    </row>
-    <row r="41" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="81" t="s">
-        <v>130</v>
-      </c>
-      <c r="B41" s="79"/>
-    </row>
-    <row r="42" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="81" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" s="79"/>
-    </row>
-    <row r="43" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="81" t="s">
-        <v>132</v>
-      </c>
-      <c r="B43" s="79"/>
-    </row>
-    <row r="44" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="81" t="s">
+    <row r="46" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="B44" s="79"/>
-    </row>
-    <row r="45" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="81" t="s">
+      <c r="B46" s="93" t="s">
+        <v>239</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B45" s="79"/>
-    </row>
-    <row r="46" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="81" t="s">
+      <c r="B47" s="125" t="s">
+        <v>240</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="79"/>
-    </row>
-    <row r="47" spans="1:2" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="82" t="s">
+      <c r="B48" s="125" t="s">
+        <v>242</v>
+      </c>
+      <c r="C48" s="117" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="74.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="99" t="s">
         <v>136</v>
       </c>
-      <c r="B47" s="80"/>
-    </row>
+      <c r="B49" s="126" t="s">
+        <v>241</v>
+      </c>
+      <c r="C49" s="118" t="s">
+        <v>191</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A39:B39"/>
+  <mergeCells count="6">
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="L18:L20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mie à jour Q et excel et sommaire
</commit_message>
<xml_diff>
--- a/REAC_Comp.xlsx
+++ b/REAC_Comp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril\DossierPerso\Document Important\école sup\Dossier_prof\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8B022D-E19D-446E-A88F-741E4A4BFF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC4137B-20AC-461E-9E70-105B8CC77B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-4680" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B7C02CEF-25C9-4280-8BD4-DADB43DFD29C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="246">
   <si>
     <t>A2T2S3 – Management des processus S.I.</t>
   </si>
@@ -816,6 +816,10 @@
   </si>
   <si>
     <t>MAIS en vrai parler des choses à améliorer dans l'équipes ? (rédaction US, TMA, …)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Demadner à Laurent/Aurélien ??</t>
   </si>
 </sst>
 </file>
@@ -1704,7 +1708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1832,6 +1836,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1910,178 +2046,37 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2111,8 +2106,8 @@
       <xdr:rowOff>587828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>18680</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>308240</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>475192</xdr:rowOff>
     </xdr:to>
@@ -2491,7 +2486,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="77" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2511,8 +2506,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69"/>
-      <c r="B3" s="71" t="s">
+      <c r="A3" s="77"/>
+      <c r="B3" s="72" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -2529,8 +2524,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="69"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="73"/>
       <c r="C4" s="17" t="s">
         <v>37</v>
       </c>
@@ -2543,8 +2538,8 @@
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="69"/>
-      <c r="B5" s="72"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="73"/>
       <c r="C5" s="17" t="s">
         <v>39</v>
       </c>
@@ -2557,8 +2552,8 @@
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69"/>
-      <c r="B6" s="73"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="18" t="s">
         <v>41</v>
       </c>
@@ -2571,8 +2566,8 @@
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="69"/>
-      <c r="B7" s="71" t="s">
+      <c r="A7" s="77"/>
+      <c r="B7" s="72" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -2587,35 +2582,35 @@
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="69"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="83" t="s">
+      <c r="A8" s="77"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="86" t="s">
+      <c r="E8" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="87"/>
+      <c r="F8" s="76"/>
     </row>
     <row r="9" spans="1:6" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="70"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="87"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
     </row>
     <row r="10" spans="1:6" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="83" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="39" t="s">
@@ -2629,9 +2624,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="78"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="35" t="s">
         <v>50</v>
       </c>
@@ -2643,8 +2638,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="69"/>
-      <c r="B12" s="76"/>
+      <c r="A12" s="77"/>
+      <c r="B12" s="82"/>
       <c r="C12" s="18" t="s">
         <v>51</v>
       </c>
@@ -2659,8 +2654,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="69"/>
-      <c r="B13" s="80" t="s">
+      <c r="A13" s="77"/>
+      <c r="B13" s="86" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -2677,9 +2672,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="69"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="78" t="s">
+      <c r="A14" s="77"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="84" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="35" t="s">
@@ -2693,9 +2688,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="69"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="78"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="35" t="s">
         <v>58</v>
       </c>
@@ -2707,9 +2702,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="69"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="78"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="84"/>
       <c r="D16" s="35" t="s">
         <v>59</v>
       </c>
@@ -2721,8 +2716,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="70"/>
-      <c r="B17" s="75"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="19" t="s">
         <v>0</v>
       </c>
@@ -2737,13 +2732,13 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="57.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="62"/>
+      <c r="C18" s="106"/>
       <c r="D18" s="34" t="s">
         <v>4</v>
       </c>
@@ -2755,9 +2750,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="47"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="66"/>
+      <c r="A19" s="91"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="110"/>
       <c r="D19" s="38" t="s">
         <v>5</v>
       </c>
@@ -2769,11 +2764,11 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="86.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="47"/>
-      <c r="B20" s="67" t="s">
+      <c r="A20" s="91"/>
+      <c r="B20" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="68"/>
+      <c r="C20" s="112"/>
       <c r="D20" s="40" t="s">
         <v>7</v>
       </c>
@@ -2785,11 +2780,11 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="47"/>
-      <c r="B21" s="49" t="s">
+      <c r="A21" s="91"/>
+      <c r="B21" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="50"/>
+      <c r="C21" s="94"/>
       <c r="D21" s="34" t="s">
         <v>9</v>
       </c>
@@ -2797,9 +2792,9 @@
       <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="47"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="52"/>
+      <c r="A22" s="91"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="96"/>
       <c r="D22" s="35" t="s">
         <v>10</v>
       </c>
@@ -2811,9 +2806,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="47"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="52"/>
+      <c r="A23" s="91"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="96"/>
       <c r="D23" s="35" t="s">
         <v>11</v>
       </c>
@@ -2825,9 +2820,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="47"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
+      <c r="A24" s="91"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="96"/>
       <c r="D24" s="35" t="s">
         <v>12</v>
       </c>
@@ -2839,9 +2834,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="48"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="54"/>
+      <c r="A25" s="92"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="98"/>
       <c r="D25" s="41" t="s">
         <v>13</v>
       </c>
@@ -2853,13 +2848,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="56"/>
+      <c r="C26" s="100"/>
       <c r="D26" s="39" t="s">
         <v>89</v>
       </c>
@@ -2871,9 +2866,9 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="58"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="101"/>
+      <c r="C27" s="102"/>
       <c r="D27" s="35" t="s">
         <v>16</v>
       </c>
@@ -2885,9 +2880,9 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="43"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="60"/>
+      <c r="A28" s="87"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="104"/>
       <c r="D28" s="36" t="s">
         <v>17</v>
       </c>
@@ -2899,11 +2894,11 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="43"/>
-      <c r="B29" s="61" t="s">
+      <c r="A29" s="87"/>
+      <c r="B29" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="62"/>
+      <c r="C29" s="106"/>
       <c r="D29" s="34" t="s">
         <v>19</v>
       </c>
@@ -2913,9 +2908,9 @@
       <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="43"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="60"/>
+      <c r="A30" s="87"/>
+      <c r="B30" s="103"/>
+      <c r="C30" s="104"/>
       <c r="D30" s="36" t="s">
         <v>20</v>
       </c>
@@ -2927,11 +2922,11 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="43"/>
-      <c r="B31" s="61" t="s">
+      <c r="A31" s="87"/>
+      <c r="B31" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="62"/>
+      <c r="C31" s="106"/>
       <c r="D31" s="34" t="s">
         <v>22</v>
       </c>
@@ -2943,9 +2938,9 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="43"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="60"/>
+      <c r="A32" s="87"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="104"/>
       <c r="D32" s="36" t="s">
         <v>23</v>
       </c>
@@ -2957,11 +2952,11 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="43"/>
-      <c r="B33" s="61" t="s">
+      <c r="A33" s="87"/>
+      <c r="B33" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="62"/>
+      <c r="C33" s="106"/>
       <c r="D33" s="34" t="s">
         <v>25</v>
       </c>
@@ -2971,9 +2966,9 @@
       <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="44"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="64"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="107"/>
+      <c r="C34" s="108"/>
       <c r="D34" s="41" t="s">
         <v>26</v>
       </c>
@@ -2985,13 +2980,13 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="52"/>
+      <c r="C35" s="96"/>
       <c r="D35" s="42" t="s">
         <v>29</v>
       </c>
@@ -3003,9 +2998,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="43"/>
-      <c r="B36" s="51"/>
-      <c r="C36" s="52"/>
+      <c r="A36" s="87"/>
+      <c r="B36" s="95"/>
+      <c r="C36" s="96"/>
       <c r="D36" s="35" t="s">
         <v>30</v>
       </c>
@@ -3017,9 +3012,9 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="43"/>
-      <c r="B37" s="51"/>
-      <c r="C37" s="52"/>
+      <c r="A37" s="87"/>
+      <c r="B37" s="95"/>
+      <c r="C37" s="96"/>
       <c r="D37" s="35" t="s">
         <v>31</v>
       </c>
@@ -3031,9 +3026,9 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="44"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="54"/>
+      <c r="A38" s="88"/>
+      <c r="B38" s="97"/>
+      <c r="C38" s="98"/>
       <c r="D38" s="41" t="s">
         <v>32</v>
       </c>
@@ -3047,18 +3042,6 @@
     <row r="39" spans="1:6" ht="24" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="C14:C16"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A26:A34"/>
     <mergeCell ref="A18:A25"/>
@@ -3070,6 +3053,18 @@
     <mergeCell ref="B35:C38"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3080,26 +3075,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D8D677-BCDB-47D5-ABA2-09C3D35E14AC}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="92.77734375" style="21" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="96" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="45" customWidth="1"/>
     <col min="3" max="3" width="61.44140625" style="21" customWidth="1"/>
     <col min="4" max="4" width="40.5546875" style="21" customWidth="1"/>
     <col min="5" max="5" width="47.88671875" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="10.88671875" style="21"/>
+    <col min="6" max="6" width="17.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.88671875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="93.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="120" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="103"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="2" spans="1:13" ht="59.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
@@ -3130,7 +3126,7 @@
       <c r="B4" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="C4" s="122" t="s">
+      <c r="C4" s="63" t="s">
         <v>243</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -3144,7 +3140,7 @@
       <c r="B5" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="C5" s="122" t="s">
+      <c r="C5" s="63" t="s">
         <v>243</v>
       </c>
       <c r="D5" s="27" t="s">
@@ -3158,10 +3154,10 @@
       <c r="B6" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="C6" s="122" t="s">
+      <c r="C6" s="63" t="s">
         <v>243</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="21" t="s">
         <v>137</v>
       </c>
       <c r="E6" s="21" t="s">
@@ -3178,13 +3174,13 @@
       <c r="B7" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="C7" s="122" t="s">
+      <c r="C7" s="63" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="90" t="s">
+      <c r="D7" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="E7" s="90" t="s">
+      <c r="E7" s="21" t="s">
         <v>159</v>
       </c>
       <c r="F7" s="26" t="s">
@@ -3192,70 +3188,47 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="88.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="123" t="s">
+      <c r="B8" s="64" t="s">
         <v>224</v>
       </c>
-      <c r="C8" s="120" t="s">
+      <c r="C8" s="61" t="s">
         <v>161</v>
       </c>
-      <c r="D8" s="121" t="s">
+      <c r="D8" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
     </row>
     <row r="9" spans="1:13" ht="60.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="104"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
+      <c r="J9" s="49"/>
     </row>
     <row r="10" spans="1:13" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="53" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="106"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="90"/>
-      <c r="K10" s="90"/>
-      <c r="L10" s="90"/>
-      <c r="M10" s="90"/>
+      <c r="C10" s="50"/>
     </row>
     <row r="11" spans="1:13" ht="83.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="44" t="s">
         <v>209</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="90"/>
     </row>
     <row r="12" spans="1:13" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="93" t="s">
+      <c r="B12" s="44" t="s">
         <v>210</v>
       </c>
       <c r="C12" s="23" t="s">
@@ -3264,18 +3237,12 @@
       <c r="D12" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
     </row>
     <row r="13" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="93" t="s">
+      <c r="B13" s="44" t="s">
         <v>211</v>
       </c>
       <c r="C13" s="23" t="s">
@@ -3284,36 +3251,26 @@
       <c r="D13" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="105"/>
+      <c r="M13" s="28"/>
     </row>
     <row r="14" spans="1:13" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="93" t="s">
+      <c r="B14" s="44" t="s">
         <v>212</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="90"/>
+      <c r="L14" s="28"/>
     </row>
     <row r="15" spans="1:13" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="44" t="s">
         <v>213</v>
       </c>
       <c r="C15" s="23" t="s">
@@ -3325,18 +3282,13 @@
       <c r="E15" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="90"/>
+      <c r="L15" s="28"/>
     </row>
     <row r="16" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="93" t="s">
+      <c r="B16" s="44" t="s">
         <v>214</v>
       </c>
       <c r="C16" s="23" t="s">
@@ -3345,21 +3297,16 @@
       <c r="D16" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="H16" s="90"/>
-      <c r="I16" s="90"/>
-      <c r="J16" s="90"/>
-      <c r="K16" s="90"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="90"/>
-    </row>
-    <row r="17" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="28"/>
+    </row>
+    <row r="17" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="93" t="s">
+      <c r="B17" s="44" t="s">
         <v>215</v>
       </c>
-      <c r="C17" s="119" t="s">
+      <c r="C17" s="60" t="s">
         <v>140</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -3368,21 +3315,15 @@
       <c r="E17" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="H17" s="90"/>
-      <c r="I17" s="90"/>
-      <c r="J17" s="90"/>
-      <c r="K17" s="90"/>
-      <c r="L17" s="90"/>
-      <c r="M17" s="90"/>
-    </row>
-    <row r="18" spans="1:13" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="99" t="s">
+    </row>
+    <row r="18" spans="1:12" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="52" t="s">
         <v>163</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -3391,42 +3332,24 @@
       <c r="E18" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="H18" s="90"/>
-      <c r="I18" s="90"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="90"/>
-      <c r="L18" s="94"/>
-      <c r="M18" s="90"/>
-    </row>
-    <row r="19" spans="1:13" ht="72.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="90"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="90"/>
-      <c r="J19" s="90"/>
-      <c r="K19" s="90"/>
-      <c r="L19" s="94"/>
-      <c r="M19" s="90"/>
-    </row>
-    <row r="20" spans="1:13" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="110" t="s">
+      <c r="L18" s="116"/>
+    </row>
+    <row r="19" spans="1:12" ht="72.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L19" s="116"/>
+    </row>
+    <row r="20" spans="1:12" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="111"/>
-      <c r="C20" s="112"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="90"/>
-      <c r="J20" s="90"/>
-      <c r="K20" s="90"/>
-      <c r="L20" s="94"/>
-      <c r="M20" s="90"/>
-    </row>
-    <row r="21" spans="1:13" ht="66.599999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="118"/>
+      <c r="C20" s="119"/>
+      <c r="L20" s="116"/>
+    </row>
+    <row r="21" spans="1:12" ht="66.599999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="93" t="s">
+      <c r="B21" s="44" t="s">
         <v>202</v>
       </c>
       <c r="C21" s="24" t="s">
@@ -3435,18 +3358,12 @@
       <c r="D21" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="H21" s="90"/>
-      <c r="I21" s="90"/>
-      <c r="J21" s="90"/>
-      <c r="K21" s="90"/>
-      <c r="L21" s="90"/>
-      <c r="M21" s="90"/>
-    </row>
-    <row r="22" spans="1:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="44" t="s">
         <v>201</v>
       </c>
       <c r="C22" s="24" t="s">
@@ -3455,36 +3372,24 @@
       <c r="D22" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="H22" s="90"/>
-      <c r="I22" s="90"/>
-      <c r="J22" s="90"/>
-      <c r="K22" s="90"/>
-      <c r="L22" s="90"/>
-      <c r="M22" s="90"/>
-    </row>
-    <row r="23" spans="1:13" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:12" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="125" t="s">
+      <c r="B23" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="C23" s="124" t="s">
+      <c r="C23" s="65" t="s">
         <v>179</v>
       </c>
       <c r="D23" s="28"/>
-      <c r="H23" s="90"/>
-      <c r="I23" s="90"/>
-      <c r="J23" s="90"/>
-      <c r="K23" s="90"/>
-      <c r="L23" s="90"/>
-      <c r="M23" s="90"/>
-    </row>
-    <row r="24" spans="1:13" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:12" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="B24" s="93" t="s">
+      <c r="B24" s="44" t="s">
         <v>204</v>
       </c>
       <c r="C24" s="24" t="s">
@@ -3496,71 +3401,59 @@
       <c r="E24" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="H24" s="90"/>
-      <c r="I24" s="90"/>
-      <c r="J24" s="90"/>
-      <c r="K24" s="90"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="90"/>
-    </row>
-    <row r="25" spans="1:13" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:12" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="93" t="s">
+      <c r="B25" s="44" t="s">
         <v>205</v>
       </c>
       <c r="C25" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="94" t="s">
+      <c r="D25" s="116" t="s">
         <v>180</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="H25" s="90"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="90"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="90"/>
-    </row>
-    <row r="26" spans="1:13" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="B26" s="93" t="s">
+      <c r="B26" s="44" t="s">
         <v>206</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="D26" s="94"/>
-    </row>
-    <row r="27" spans="1:13" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="116"/>
+    </row>
+    <row r="27" spans="1:12" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="44" t="s">
         <v>207</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="D27" s="94"/>
+      <c r="D27" s="116"/>
       <c r="E27" s="28" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="99" t="s">
+    <row r="28" spans="1:12" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="B28" s="107" t="s">
+      <c r="B28" s="51" t="s">
         <v>208</v>
       </c>
-      <c r="C28" s="108" t="s">
+      <c r="C28" s="52" t="s">
         <v>150</v>
       </c>
       <c r="D28" s="21" t="s">
@@ -3570,37 +3463,34 @@
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="91"/>
-      <c r="B29" s="95"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
+    <row r="29" spans="1:12" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="43"/>
       <c r="E29" s="28"/>
     </row>
-    <row r="30" spans="1:13" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="88" t="s">
+    <row r="30" spans="1:12" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="113" t="s">
         <v>234</v>
       </c>
-      <c r="B30" s="92"/>
-      <c r="C30" s="89"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="123"/>
       <c r="E30" s="28"/>
     </row>
-    <row r="31" spans="1:13" ht="61.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="61.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="93" t="s">
+      <c r="B31" s="44" t="s">
         <v>225</v>
       </c>
       <c r="C31" s="23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="93" t="s">
+      <c r="B32" s="44" t="s">
         <v>226</v>
       </c>
       <c r="C32" s="23" t="s">
@@ -3611,7 +3501,7 @@
       <c r="A33" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="B33" s="93" t="s">
+      <c r="B33" s="44" t="s">
         <v>227</v>
       </c>
       <c r="C33" s="23" t="s">
@@ -3622,10 +3512,10 @@
       <c r="A34" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="125" t="s">
+      <c r="B34" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="C34" s="113" t="s">
+      <c r="C34" s="54" t="s">
         <v>195</v>
       </c>
       <c r="D34" s="31"/>
@@ -3634,7 +3524,7 @@
       <c r="A35" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="B35" s="93" t="s">
+      <c r="B35" s="44" t="s">
         <v>228</v>
       </c>
       <c r="C35" s="23" t="s">
@@ -3645,7 +3535,7 @@
       <c r="A36" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="B36" s="93" t="s">
+      <c r="B36" s="44" t="s">
         <v>230</v>
       </c>
       <c r="C36" s="23" t="s">
@@ -3656,10 +3546,10 @@
       <c r="A37" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="125" t="s">
+      <c r="B37" s="66" t="s">
         <v>231</v>
       </c>
-      <c r="C37" s="114" t="s">
+      <c r="C37" s="55" t="s">
         <v>198</v>
       </c>
       <c r="D37" s="30"/>
@@ -3668,7 +3558,7 @@
       <c r="A38" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="93" t="s">
+      <c r="B38" s="44" t="s">
         <v>232</v>
       </c>
       <c r="C38" s="23" t="s">
@@ -3676,37 +3566,34 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="99" t="s">
+      <c r="A39" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="B39" s="100" t="s">
+      <c r="B39" s="48" t="s">
         <v>233</v>
       </c>
-      <c r="C39" s="115" t="s">
+      <c r="C39" s="56" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="69" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="91"/>
-      <c r="B40" s="95"/>
-      <c r="C40" s="90"/>
-      <c r="D40" s="90"/>
+      <c r="A40" s="43"/>
     </row>
     <row r="41" spans="1:4" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="88" t="s">
+      <c r="A41" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="92"/>
-      <c r="C41" s="97"/>
+      <c r="B41" s="114"/>
+      <c r="C41" s="115"/>
     </row>
     <row r="42" spans="1:4" ht="66.599999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="B42" s="93" t="s">
+      <c r="B42" s="44" t="s">
         <v>235</v>
       </c>
-      <c r="C42" s="98" t="s">
+      <c r="C42" s="46" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3714,7 +3601,7 @@
       <c r="A43" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="93" t="s">
+      <c r="B43" s="44" t="s">
         <v>236</v>
       </c>
       <c r="C43" s="24" t="s">
@@ -3725,7 +3612,7 @@
       <c r="A44" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="93" t="s">
+      <c r="B44" s="44" t="s">
         <v>237</v>
       </c>
       <c r="C44" s="24" t="s">
@@ -3739,10 +3626,10 @@
       <c r="A45" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="125" t="s">
+      <c r="B45" s="66" t="s">
         <v>238</v>
       </c>
-      <c r="C45" s="116" t="s">
+      <c r="C45" s="57" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3750,7 +3637,7 @@
       <c r="A46" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="B46" s="93" t="s">
+      <c r="B46" s="44" t="s">
         <v>239</v>
       </c>
       <c r="C46" s="24" t="s">
@@ -3761,7 +3648,7 @@
       <c r="A47" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="125" t="s">
+      <c r="B47" s="66" t="s">
         <v>240</v>
       </c>
       <c r="C47" s="24" t="s">
@@ -3775,21 +3662,21 @@
       <c r="A48" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="B48" s="125" t="s">
+      <c r="B48" s="66" t="s">
         <v>242</v>
       </c>
-      <c r="C48" s="117" t="s">
+      <c r="C48" s="58" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="74.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="99" t="s">
+      <c r="A49" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="B49" s="126" t="s">
+      <c r="B49" s="67" t="s">
         <v>241</v>
       </c>
-      <c r="C49" s="118" t="s">
+      <c r="C49" s="59" t="s">
         <v>191</v>
       </c>
       <c r="D49" s="21" t="s">
@@ -3799,12 +3686,12 @@
     <row r="50" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="L18:L20"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="D25:D27"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A30:C30"/>
-    <mergeCell ref="L18:L20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
mise à jour Q Domus et ajout info
</commit_message>
<xml_diff>
--- a/REAC_Comp.xlsx
+++ b/REAC_Comp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril\DossierPerso\Document Important\école sup\Dossier_prof\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AY024303\Cyril\Doc perso\Diplome I5\Dossier_prof\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC4137B-20AC-461E-9E70-105B8CC77B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BB2B0B-E02B-4F59-AC60-6DB0D3955584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4680" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B7C02CEF-25C9-4280-8BD4-DADB43DFD29C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{B7C02CEF-25C9-4280-8BD4-DADB43DFD29C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1911,6 +1911,120 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1923,12 +2037,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1938,112 +2046,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2053,9 +2056,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2454,18 +2454,18 @@
       <selection activeCell="A18" sqref="A18:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="23.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="40.5546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="48.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40.54296875" style="3" customWidth="1"/>
     <col min="3" max="3" width="45" style="20" customWidth="1"/>
-    <col min="4" max="4" width="76.5546875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="39.21875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="1"/>
+    <col min="4" max="4" width="76.54296875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="39.1796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>64</v>
       </c>
@@ -2485,8 +2485,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="77" t="s">
+    <row r="2" spans="1:6" ht="59" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="94" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2505,9 +2505,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="72" t="s">
+    <row r="3" spans="1:6" ht="98.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="94"/>
+      <c r="B3" s="96" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -2523,9 +2523,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="77"/>
-      <c r="B4" s="73"/>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="94"/>
+      <c r="B4" s="97"/>
       <c r="C4" s="17" t="s">
         <v>37</v>
       </c>
@@ -2537,9 +2537,9 @@
       </c>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="77"/>
-      <c r="B5" s="73"/>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="94"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="17" t="s">
         <v>39</v>
       </c>
@@ -2551,9 +2551,9 @@
       </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="77"/>
-      <c r="B6" s="79"/>
+    <row r="6" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="94"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="18" t="s">
         <v>41</v>
       </c>
@@ -2565,9 +2565,9 @@
       </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="77"/>
-      <c r="B7" s="72" t="s">
+    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="94"/>
+      <c r="B7" s="96" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -2581,36 +2581,36 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="70" t="s">
+    <row r="8" spans="1:6" ht="43.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="94"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="75" t="s">
+      <c r="E8" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="76"/>
-    </row>
-    <row r="9" spans="1:6" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="78"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="76"/>
-    </row>
-    <row r="10" spans="1:6" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="85" t="s">
+      <c r="F8" s="112"/>
+    </row>
+    <row r="9" spans="1:6" ht="21.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="95"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="112"/>
+    </row>
+    <row r="10" spans="1:6" ht="44" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="104" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="83" t="s">
+      <c r="C10" s="102" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="39" t="s">
@@ -2623,10 +2623,10 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="77"/>
-      <c r="B11" s="81"/>
-      <c r="C11" s="84"/>
+    <row r="11" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="94"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="103"/>
       <c r="D11" s="35" t="s">
         <v>50</v>
       </c>
@@ -2637,9 +2637,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="77"/>
-      <c r="B12" s="82"/>
+    <row r="12" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="94"/>
+      <c r="B12" s="101"/>
       <c r="C12" s="18" t="s">
         <v>51</v>
       </c>
@@ -2653,9 +2653,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="77"/>
-      <c r="B13" s="86" t="s">
+    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="94"/>
+      <c r="B13" s="105" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -2671,10 +2671,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="77"/>
-      <c r="B14" s="81"/>
-      <c r="C14" s="84" t="s">
+    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="94"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="103" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="35" t="s">
@@ -2687,10 +2687,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="77"/>
-      <c r="B15" s="81"/>
-      <c r="C15" s="84"/>
+    <row r="15" spans="1:6" ht="53.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="94"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="35" t="s">
         <v>58</v>
       </c>
@@ -2701,10 +2701,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="77"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="84"/>
+    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="94"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="35" t="s">
         <v>59</v>
       </c>
@@ -2715,9 +2715,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="78"/>
-      <c r="B17" s="81"/>
+    <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="95"/>
+      <c r="B17" s="100"/>
       <c r="C17" s="19" t="s">
         <v>0</v>
       </c>
@@ -2731,14 +2731,14 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="57.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="90" t="s">
+    <row r="18" spans="1:6" ht="57.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="105" t="s">
+      <c r="B18" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="106"/>
+      <c r="C18" s="87"/>
       <c r="D18" s="34" t="s">
         <v>4</v>
       </c>
@@ -2749,10 +2749,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="91"/>
-      <c r="B19" s="109"/>
-      <c r="C19" s="110"/>
+    <row r="19" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="72"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="91"/>
       <c r="D19" s="38" t="s">
         <v>5</v>
       </c>
@@ -2763,12 +2763,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="86.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="91"/>
-      <c r="B20" s="111" t="s">
+    <row r="20" spans="1:6" ht="86.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="72"/>
+      <c r="B20" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="112"/>
+      <c r="C20" s="93"/>
       <c r="D20" s="40" t="s">
         <v>7</v>
       </c>
@@ -2779,22 +2779,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="91"/>
-      <c r="B21" s="93" t="s">
+    <row r="21" spans="1:6" ht="101.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="72"/>
+      <c r="B21" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="94"/>
+      <c r="C21" s="75"/>
       <c r="D21" s="34" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="91"/>
-      <c r="B22" s="95"/>
-      <c r="C22" s="96"/>
+    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="72"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="77"/>
       <c r="D22" s="35" t="s">
         <v>10</v>
       </c>
@@ -2805,10 +2805,10 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="91"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="96"/>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="72"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="77"/>
       <c r="D23" s="35" t="s">
         <v>11</v>
       </c>
@@ -2819,10 +2819,10 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="91"/>
-      <c r="B24" s="95"/>
-      <c r="C24" s="96"/>
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="72"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="77"/>
       <c r="D24" s="35" t="s">
         <v>12</v>
       </c>
@@ -2833,10 +2833,10 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="92"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="98"/>
+    <row r="25" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="73"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="79"/>
       <c r="D25" s="41" t="s">
         <v>13</v>
       </c>
@@ -2847,14 +2847,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="89" t="s">
+    <row r="26" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="99" t="s">
+      <c r="B26" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="100"/>
+      <c r="C26" s="81"/>
       <c r="D26" s="39" t="s">
         <v>89</v>
       </c>
@@ -2865,10 +2865,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="87"/>
-      <c r="B27" s="101"/>
-      <c r="C27" s="102"/>
+    <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="68"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="83"/>
       <c r="D27" s="35" t="s">
         <v>16</v>
       </c>
@@ -2879,10 +2879,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="87"/>
-      <c r="B28" s="103"/>
-      <c r="C28" s="104"/>
+    <row r="28" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="68"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="36" t="s">
         <v>17</v>
       </c>
@@ -2893,12 +2893,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="87"/>
-      <c r="B29" s="105" t="s">
+    <row r="29" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="68"/>
+      <c r="B29" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="106"/>
+      <c r="C29" s="87"/>
       <c r="D29" s="34" t="s">
         <v>19</v>
       </c>
@@ -2907,10 +2907,10 @@
       </c>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="87"/>
-      <c r="B30" s="103"/>
-      <c r="C30" s="104"/>
+    <row r="30" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="68"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="36" t="s">
         <v>20</v>
       </c>
@@ -2921,12 +2921,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="87"/>
-      <c r="B31" s="105" t="s">
+    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="68"/>
+      <c r="B31" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="106"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="34" t="s">
         <v>22</v>
       </c>
@@ -2937,10 +2937,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="87"/>
-      <c r="B32" s="103"/>
-      <c r="C32" s="104"/>
+    <row r="32" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="68"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="85"/>
       <c r="D32" s="36" t="s">
         <v>23</v>
       </c>
@@ -2951,12 +2951,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="87"/>
-      <c r="B33" s="105" t="s">
+    <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="68"/>
+      <c r="B33" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="106"/>
+      <c r="C33" s="87"/>
       <c r="D33" s="34" t="s">
         <v>25</v>
       </c>
@@ -2965,10 +2965,10 @@
       </c>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="88"/>
-      <c r="B34" s="107"/>
-      <c r="C34" s="108"/>
+    <row r="34" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="69"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="89"/>
       <c r="D34" s="41" t="s">
         <v>26</v>
       </c>
@@ -2979,14 +2979,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="87" t="s">
+    <row r="35" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="95" t="s">
+      <c r="B35" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="96"/>
+      <c r="C35" s="77"/>
       <c r="D35" s="42" t="s">
         <v>29</v>
       </c>
@@ -2997,10 +2997,10 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="87"/>
-      <c r="B36" s="95"/>
-      <c r="C36" s="96"/>
+    <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="68"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="77"/>
       <c r="D36" s="35" t="s">
         <v>30</v>
       </c>
@@ -3011,10 +3011,10 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="87"/>
-      <c r="B37" s="95"/>
-      <c r="C37" s="96"/>
+    <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="68"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="77"/>
       <c r="D37" s="35" t="s">
         <v>31</v>
       </c>
@@ -3025,10 +3025,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="88"/>
-      <c r="B38" s="97"/>
-      <c r="C38" s="98"/>
+    <row r="38" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="69"/>
+      <c r="B38" s="78"/>
+      <c r="C38" s="79"/>
       <c r="D38" s="41" t="s">
         <v>32</v>
       </c>
@@ -3039,9 +3039,21 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="24" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:6" ht="24" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="C14:C16"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A26:A34"/>
     <mergeCell ref="A18:A25"/>
@@ -3053,18 +3065,6 @@
     <mergeCell ref="B35:C38"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3075,29 +3075,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D8D677-BCDB-47D5-ABA2-09C3D35E14AC}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.77734375" style="21" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="45" customWidth="1"/>
-    <col min="3" max="3" width="61.44140625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="47.88671875" style="21" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.88671875" style="21"/>
+    <col min="1" max="1" width="92.81640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" style="45" customWidth="1"/>
+    <col min="3" max="3" width="61.453125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="40.54296875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="47.90625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.90625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="93.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="93.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="120" t="s">
         <v>217</v>
       </c>
       <c r="B1" s="121"/>
       <c r="C1" s="122"/>
     </row>
-    <row r="2" spans="1:13" ht="59.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="59.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>100</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="24" t="s">
         <v>101</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="104.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
         <v>102</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
         <v>103</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="109.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
         <v>104</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="81.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>105</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="88.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="88" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="47" t="s">
         <v>106</v>
       </c>
@@ -3201,10 +3201,10 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="60.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="60.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J9" s="49"/>
     </row>
-    <row r="10" spans="1:13" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="42.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="53" t="s">
         <v>62</v>
       </c>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="C10" s="50"/>
     </row>
-    <row r="11" spans="1:13" ht="83.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="83.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>141</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="s">
         <v>111</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>112</v>
       </c>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="M13" s="28"/>
     </row>
-    <row r="14" spans="1:13" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
         <v>113</v>
       </c>
@@ -3266,7 +3266,7 @@
       </c>
       <c r="L14" s="28"/>
     </row>
-    <row r="15" spans="1:13" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="79.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
         <v>107</v>
       </c>
@@ -3284,7 +3284,7 @@
       </c>
       <c r="L15" s="28"/>
     </row>
-    <row r="16" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>108</v>
       </c>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="L16" s="28"/>
     </row>
-    <row r="17" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
         <v>109</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="47" t="s">
         <v>110</v>
       </c>
@@ -3332,20 +3332,20 @@
       <c r="E18" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L18" s="116"/>
-    </row>
-    <row r="19" spans="1:12" ht="72.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L19" s="116"/>
-    </row>
-    <row r="20" spans="1:12" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L18" s="113"/>
+    </row>
+    <row r="19" spans="1:12" ht="72.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L19" s="113"/>
+    </row>
+    <row r="20" spans="1:12" ht="79.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="117" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="118"/>
       <c r="C20" s="119"/>
-      <c r="L20" s="116"/>
-    </row>
-    <row r="21" spans="1:12" ht="66.599999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="113"/>
+    </row>
+    <row r="21" spans="1:12" ht="66.650000000000006" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A21" s="24" t="s">
         <v>114</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
         <v>115</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="24" t="s">
         <v>116</v>
       </c>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="D23" s="28"/>
     </row>
-    <row r="24" spans="1:12" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="73.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="24" t="s">
         <v>117</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="86.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="24" t="s">
         <v>118</v>
       </c>
@@ -3412,14 +3412,14 @@
       <c r="C25" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="116" t="s">
+      <c r="D25" s="113" t="s">
         <v>180</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="55.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="24" t="s">
         <v>119</v>
       </c>
@@ -3429,9 +3429,9 @@
       <c r="C26" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="D26" s="116"/>
-    </row>
-    <row r="27" spans="1:12" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="113"/>
+    </row>
+    <row r="27" spans="1:12" ht="76.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="24" t="s">
         <v>120</v>
       </c>
@@ -3441,12 +3441,12 @@
       <c r="C27" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="D27" s="116"/>
+      <c r="D27" s="113"/>
       <c r="E27" s="28" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="47" t="s">
         <v>121</v>
       </c>
@@ -3463,19 +3463,19 @@
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="42.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="43"/>
       <c r="E29" s="28"/>
     </row>
-    <row r="30" spans="1:12" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="113" t="s">
+    <row r="30" spans="1:12" ht="42.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="114" t="s">
         <v>234</v>
       </c>
-      <c r="B30" s="114"/>
+      <c r="B30" s="115"/>
       <c r="C30" s="123"/>
       <c r="E30" s="28"/>
     </row>
-    <row r="31" spans="1:12" ht="61.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="61.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A31" s="24" t="s">
         <v>122</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="88.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="24" t="s">
         <v>123</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="82.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="24" t="s">
         <v>124</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="24" t="s">
         <v>125</v>
       </c>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="D34" s="31"/>
     </row>
-    <row r="35" spans="1:4" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="24" t="s">
         <v>126</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="24" t="s">
         <v>151</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="24" t="s">
         <v>127</v>
       </c>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="D37" s="30"/>
     </row>
-    <row r="38" spans="1:4" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="76.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="24" t="s">
         <v>128</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="47" t="s">
         <v>129</v>
       </c>
@@ -3576,17 +3576,17 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="69" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="69" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="43"/>
     </row>
-    <row r="41" spans="1:4" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="113" t="s">
+    <row r="41" spans="1:4" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="114"/>
-      <c r="C41" s="115"/>
-    </row>
-    <row r="42" spans="1:4" ht="66.599999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="115"/>
+      <c r="C41" s="116"/>
+    </row>
+    <row r="42" spans="1:4" ht="66.650000000000006" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A42" s="24" t="s">
         <v>152</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="24" t="s">
         <v>130</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="61.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="24" t="s">
         <v>131</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="85.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="24" t="s">
         <v>132</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="24" t="s">
         <v>133</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="24" t="s">
         <v>134</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="24" t="s">
         <v>135</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="74.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="74.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="47" t="s">
         <v>136</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="L18:L20"/>

</xml_diff>

<commit_message>
fuck finish 2h plus tard à cause word de merde
</commit_message>
<xml_diff>
--- a/REAC_Comp.xlsx
+++ b/REAC_Comp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril\DossierPerso\Document Important\école sup\Dossier_prof\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AY024303\Cyril\Doc perso\Diplome I5\Dossier_prof\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C692D6B-6E60-44DF-A502-0FCBD743B27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0E93CC-4B39-4EC4-8721-039C0C07950D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{B7C02CEF-25C9-4280-8BD4-DADB43DFD29C}"/>
+    <workbookView xWindow="28800" yWindow="-4170" windowWidth="14400" windowHeight="16200" activeTab="1" xr2:uid="{B7C02CEF-25C9-4280-8BD4-DADB43DFD29C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2318,6 +2318,120 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2330,12 +2444,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2343,114 +2451,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2861,18 +2861,18 @@
       <selection activeCell="A18" sqref="A18:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="23.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="40.5546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="48.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40.54296875" style="3" customWidth="1"/>
     <col min="3" max="3" width="45" style="20" customWidth="1"/>
-    <col min="4" max="4" width="76.5546875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="39.21875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="1"/>
+    <col min="4" max="4" width="76.54296875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="39.1796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>64</v>
       </c>
@@ -2892,8 +2892,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="80" t="s">
+    <row r="2" spans="1:6" ht="59" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="97" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2912,9 +2912,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="80"/>
-      <c r="B3" s="75" t="s">
+    <row r="3" spans="1:6" ht="98.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="97"/>
+      <c r="B3" s="99" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -2930,9 +2930,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="80"/>
-      <c r="B4" s="76"/>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="97"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="17" t="s">
         <v>37</v>
       </c>
@@ -2944,9 +2944,9 @@
       </c>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="80"/>
-      <c r="B5" s="76"/>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="97"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="17" t="s">
         <v>39</v>
       </c>
@@ -2958,9 +2958,9 @@
       </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="80"/>
-      <c r="B6" s="82"/>
+    <row r="6" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="97"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="18" t="s">
         <v>41</v>
       </c>
@@ -2972,9 +2972,9 @@
       </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="80"/>
-      <c r="B7" s="75" t="s">
+    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="97"/>
+      <c r="B7" s="99" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -2988,36 +2988,36 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="73" t="s">
+    <row r="8" spans="1:6" ht="43.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="97"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="111" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="109" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="78" t="s">
+      <c r="E8" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="79"/>
-    </row>
-    <row r="9" spans="1:6" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="81"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="79"/>
-    </row>
-    <row r="10" spans="1:6" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="88" t="s">
+      <c r="F8" s="115"/>
+    </row>
+    <row r="9" spans="1:6" ht="21.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="98"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="115"/>
+    </row>
+    <row r="10" spans="1:6" ht="44" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="105" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="35" t="s">
@@ -3030,10 +3030,10 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="80"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="87"/>
+    <row r="11" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="97"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="106"/>
       <c r="D11" s="31" t="s">
         <v>50</v>
       </c>
@@ -3044,9 +3044,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="80"/>
-      <c r="B12" s="85"/>
+    <row r="12" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="97"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="18" t="s">
         <v>51</v>
       </c>
@@ -3060,9 +3060,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="80"/>
-      <c r="B13" s="89" t="s">
+    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="97"/>
+      <c r="B13" s="108" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -3078,10 +3078,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="80"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="87" t="s">
+    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="97"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="106" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="31" t="s">
@@ -3094,10 +3094,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="87"/>
+    <row r="15" spans="1:6" ht="53.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="97"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="106"/>
       <c r="D15" s="31" t="s">
         <v>58</v>
       </c>
@@ -3108,10 +3108,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="80"/>
-      <c r="B16" s="84"/>
-      <c r="C16" s="87"/>
+    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="97"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="106"/>
       <c r="D16" s="31" t="s">
         <v>59</v>
       </c>
@@ -3122,9 +3122,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="81"/>
-      <c r="B17" s="84"/>
+    <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="98"/>
+      <c r="B17" s="103"/>
       <c r="C17" s="19" t="s">
         <v>0</v>
       </c>
@@ -3138,14 +3138,14 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="57.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="93" t="s">
+    <row r="18" spans="1:6" ht="57.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="108" t="s">
+      <c r="B18" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="109"/>
+      <c r="C18" s="90"/>
       <c r="D18" s="30" t="s">
         <v>4</v>
       </c>
@@ -3156,10 +3156,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="94"/>
-      <c r="B19" s="112"/>
-      <c r="C19" s="113"/>
+    <row r="19" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="75"/>
+      <c r="B19" s="93"/>
+      <c r="C19" s="94"/>
       <c r="D19" s="34" t="s">
         <v>5</v>
       </c>
@@ -3170,12 +3170,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="86.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="94"/>
-      <c r="B20" s="114" t="s">
+    <row r="20" spans="1:6" ht="86.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="75"/>
+      <c r="B20" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="115"/>
+      <c r="C20" s="96"/>
       <c r="D20" s="36" t="s">
         <v>7</v>
       </c>
@@ -3186,22 +3186,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="94"/>
-      <c r="B21" s="96" t="s">
+    <row r="21" spans="1:6" ht="101.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="75"/>
+      <c r="B21" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="97"/>
+      <c r="C21" s="78"/>
       <c r="D21" s="30" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="94"/>
-      <c r="B22" s="98"/>
-      <c r="C22" s="99"/>
+    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="75"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="31" t="s">
         <v>10</v>
       </c>
@@ -3212,10 +3212,10 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="94"/>
-      <c r="B23" s="98"/>
-      <c r="C23" s="99"/>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="75"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="80"/>
       <c r="D23" s="31" t="s">
         <v>11</v>
       </c>
@@ -3226,10 +3226,10 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="94"/>
-      <c r="B24" s="98"/>
-      <c r="C24" s="99"/>
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="75"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="80"/>
       <c r="D24" s="31" t="s">
         <v>12</v>
       </c>
@@ -3240,10 +3240,10 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="95"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="101"/>
+    <row r="25" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="76"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="82"/>
       <c r="D25" s="37" t="s">
         <v>13</v>
       </c>
@@ -3254,14 +3254,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="92" t="s">
+    <row r="26" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="102" t="s">
+      <c r="B26" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="103"/>
+      <c r="C26" s="84"/>
       <c r="D26" s="35" t="s">
         <v>89</v>
       </c>
@@ -3272,10 +3272,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="90"/>
-      <c r="B27" s="104"/>
-      <c r="C27" s="105"/>
+    <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="71"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="86"/>
       <c r="D27" s="31" t="s">
         <v>16</v>
       </c>
@@ -3286,10 +3286,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="90"/>
-      <c r="B28" s="106"/>
-      <c r="C28" s="107"/>
+    <row r="28" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="71"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="88"/>
       <c r="D28" s="32" t="s">
         <v>17</v>
       </c>
@@ -3300,12 +3300,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="90"/>
-      <c r="B29" s="108" t="s">
+    <row r="29" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="71"/>
+      <c r="B29" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="109"/>
+      <c r="C29" s="90"/>
       <c r="D29" s="30" t="s">
         <v>19</v>
       </c>
@@ -3314,10 +3314,10 @@
       </c>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="90"/>
-      <c r="B30" s="106"/>
-      <c r="C30" s="107"/>
+    <row r="30" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="71"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="88"/>
       <c r="D30" s="32" t="s">
         <v>20</v>
       </c>
@@ -3328,12 +3328,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="90"/>
-      <c r="B31" s="108" t="s">
+    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="71"/>
+      <c r="B31" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="109"/>
+      <c r="C31" s="90"/>
       <c r="D31" s="30" t="s">
         <v>22</v>
       </c>
@@ -3344,10 +3344,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="90"/>
-      <c r="B32" s="106"/>
-      <c r="C32" s="107"/>
+    <row r="32" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="71"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="88"/>
       <c r="D32" s="32" t="s">
         <v>23</v>
       </c>
@@ -3358,12 +3358,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="90"/>
-      <c r="B33" s="108" t="s">
+    <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="71"/>
+      <c r="B33" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="109"/>
+      <c r="C33" s="90"/>
       <c r="D33" s="30" t="s">
         <v>25</v>
       </c>
@@ -3372,10 +3372,10 @@
       </c>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="91"/>
-      <c r="B34" s="110"/>
-      <c r="C34" s="111"/>
+    <row r="34" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="72"/>
+      <c r="B34" s="91"/>
+      <c r="C34" s="92"/>
       <c r="D34" s="37" t="s">
         <v>26</v>
       </c>
@@ -3386,14 +3386,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="90" t="s">
+    <row r="35" spans="1:6" ht="86.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="98" t="s">
+      <c r="B35" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="99"/>
+      <c r="C35" s="80"/>
       <c r="D35" s="38" t="s">
         <v>29</v>
       </c>
@@ -3404,10 +3404,10 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="90"/>
-      <c r="B36" s="98"/>
-      <c r="C36" s="99"/>
+    <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="71"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="80"/>
       <c r="D36" s="31" t="s">
         <v>30</v>
       </c>
@@ -3418,10 +3418,10 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="90"/>
-      <c r="B37" s="98"/>
-      <c r="C37" s="99"/>
+    <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="71"/>
+      <c r="B37" s="79"/>
+      <c r="C37" s="80"/>
       <c r="D37" s="31" t="s">
         <v>31</v>
       </c>
@@ -3432,10 +3432,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="91"/>
-      <c r="B38" s="100"/>
-      <c r="C38" s="101"/>
+    <row r="38" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="72"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="82"/>
       <c r="D38" s="37" t="s">
         <v>32</v>
       </c>
@@ -3446,9 +3446,21 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="24" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:6" ht="24" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="C14:C16"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A26:A34"/>
     <mergeCell ref="A18:A25"/>
@@ -3460,18 +3472,6 @@
     <mergeCell ref="B35:C38"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3482,29 +3482,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D8D677-BCDB-47D5-ABA2-09C3D35E14AC}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="25.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="26" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.77734375" style="67" customWidth="1"/>
+    <col min="1" max="1" width="92.81640625" style="67" customWidth="1"/>
     <col min="2" max="2" width="24" style="43" customWidth="1"/>
-    <col min="3" max="3" width="94.6640625" style="53" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="47.88671875" style="21" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.88671875" style="21"/>
+    <col min="3" max="3" width="94.6328125" style="53" customWidth="1"/>
+    <col min="4" max="4" width="40.54296875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="47.90625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.90625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="93.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="93.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="123" t="s">
         <v>195</v>
       </c>
       <c r="B1" s="124"/>
       <c r="C1" s="125"/>
     </row>
-    <row r="2" spans="1:13" ht="127.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="127.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="65" t="s">
         <v>100</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="121.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="65" t="s">
         <v>101</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="104.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="65" t="s">
         <v>102</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="65" t="s">
         <v>103</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="109.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="65" t="s">
         <v>104</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="98.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="65" t="s">
         <v>105</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="88.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="88" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="66" t="s">
         <v>106</v>
       </c>
@@ -3611,10 +3611,10 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="60.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="60.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J9" s="39"/>
     </row>
-    <row r="10" spans="1:13" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="42.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="68" t="s">
         <v>62</v>
       </c>
@@ -3623,7 +3623,7 @@
       </c>
       <c r="C10" s="54"/>
     </row>
-    <row r="11" spans="1:13" ht="128.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="128.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A11" s="65" t="s">
         <v>139</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="65" t="s">
         <v>111</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="73.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="65" t="s">
         <v>112</v>
       </c>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="M13" s="25"/>
     </row>
-    <row r="14" spans="1:13" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="106.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="65" t="s">
         <v>113</v>
       </c>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="L14" s="25"/>
     </row>
-    <row r="15" spans="1:13" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="150" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="65" t="s">
         <v>107</v>
       </c>
@@ -3696,7 +3696,7 @@
       </c>
       <c r="L15" s="25"/>
     </row>
-    <row r="16" spans="1:13" ht="129" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="130" x14ac:dyDescent="0.35">
       <c r="A16" s="65" t="s">
         <v>108</v>
       </c>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="L16" s="25"/>
     </row>
-    <row r="17" spans="1:12" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="86.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="65" t="s">
         <v>109</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="77.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="66" t="s">
         <v>110</v>
       </c>
@@ -3746,10 +3746,10 @@
       </c>
       <c r="L18" s="116"/>
     </row>
-    <row r="19" spans="1:12" ht="72.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="72.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="L19" s="116"/>
     </row>
-    <row r="20" spans="1:12" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="79.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="120" t="s">
         <v>2</v>
       </c>
@@ -3757,7 +3757,7 @@
       <c r="C20" s="122"/>
       <c r="L20" s="116"/>
     </row>
-    <row r="21" spans="1:12" ht="66.599999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="66.650000000000006" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A21" s="65" t="s">
         <v>114</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="109.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="65" t="s">
         <v>115</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="65" t="s">
         <v>116</v>
       </c>
@@ -3797,7 +3797,7 @@
       </c>
       <c r="D23" s="25"/>
     </row>
-    <row r="24" spans="1:12" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="73.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="65" t="s">
         <v>117</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="86.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="65" t="s">
         <v>118</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="55.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="65" t="s">
         <v>119</v>
       </c>
@@ -3843,7 +3843,7 @@
       </c>
       <c r="D26" s="116"/>
     </row>
-    <row r="27" spans="1:12" ht="125.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="125.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="65" t="s">
         <v>120</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="66" t="s">
         <v>121</v>
       </c>
@@ -3875,11 +3875,11 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="42.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="69"/>
       <c r="E29" s="25"/>
     </row>
-    <row r="30" spans="1:12" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="42.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="117" t="s">
         <v>212</v>
       </c>
@@ -3887,7 +3887,7 @@
       <c r="C30" s="126"/>
       <c r="E30" s="25"/>
     </row>
-    <row r="31" spans="1:12" ht="61.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="61.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A31" s="65" t="s">
         <v>122</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="88.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="65" t="s">
         <v>123</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="82.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="65" t="s">
         <v>124</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="65" t="s">
         <v>125</v>
       </c>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="D34" s="27"/>
     </row>
-    <row r="35" spans="1:4" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="79.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="65" t="s">
         <v>126</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="65" t="s">
         <v>141</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="60.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="65" t="s">
         <v>127</v>
       </c>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="D37" s="26"/>
     </row>
-    <row r="38" spans="1:4" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="76.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="65" t="s">
         <v>128</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="66" t="s">
         <v>129</v>
       </c>
@@ -3988,17 +3988,17 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="69" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="69" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="69"/>
     </row>
-    <row r="41" spans="1:4" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="117" t="s">
         <v>27</v>
       </c>
       <c r="B41" s="118"/>
       <c r="C41" s="119"/>
     </row>
-    <row r="42" spans="1:4" ht="90.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="90.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A42" s="65" t="s">
         <v>142</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="65" t="s">
         <v>130</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="86.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="65" t="s">
         <v>131</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="85.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="65" t="s">
         <v>132</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="65" t="s">
         <v>133</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="65" t="s">
         <v>134</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="65" t="s">
         <v>135</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="74.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="74.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="66" t="s">
         <v>136</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="26.4" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:4" ht="26.5" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="L18:L20"/>

</xml_diff>